<commit_message>
- Fix major bugs
</commit_message>
<xml_diff>
--- a/Engines/Resources/2.xlsx
+++ b/Engines/Resources/2.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Info" sheetId="2" r:id="rId2"/>
-    <sheet name="DataHid" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="DataHid" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Info!$B$3:$M$69</definedName>
@@ -788,46 +788,46 @@
             <c:numRef>
               <c:f>DataHid!$C$6:$O$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-">
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3870</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5716</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6729</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5535</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5328</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4130</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>820</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7546.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11528.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10664</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10762.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11959.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,46 +929,46 @@
             <c:numRef>
               <c:f>DataHid!$C$7:$O$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-">
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>87</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>108</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>106</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,46 +1271,46 @@
             <c:numRef>
               <c:f>DataHid!$C$11:$P$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-">
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>74</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>98</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1412,46 +1412,46 @@
             <c:numRef>
               <c:f>DataHid!$C$12:$P$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-">
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>113.82352941176499</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.193548387096797</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.389610389610397</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>128.720930232558</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121.09090909090899</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98.3333333333333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>93.165432098765393</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>132.511494252874</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>98.740740740740705</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>101.53301886792499</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>99.661666666666704</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1772,25 +1772,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>106</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>77</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5448,8 +5448,8 @@
   </sheetPr>
   <dimension ref="A1:BE81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="Q18" zoomScale="265" zoomScaleSheetLayoutView="265" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24:U24"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="V67" sqref="V67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8976,7 +8976,7 @@
       <c r="D59" s="4"/>
       <c r="E59" s="58"/>
       <c r="F59" s="60">
-        <v>123123</v>
+        <v>0</v>
       </c>
       <c r="G59" s="60"/>
       <c r="H59" s="60"/>
@@ -9101,7 +9101,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="58"/>
       <c r="F61" s="60">
-        <v>123123</v>
+        <v>0</v>
       </c>
       <c r="G61" s="60"/>
       <c r="H61" s="60"/>
@@ -9226,7 +9226,7 @@
       <c r="D63" s="4"/>
       <c r="E63" s="58"/>
       <c r="F63" s="60">
-        <v>213</v>
+        <v>0</v>
       </c>
       <c r="G63" s="60"/>
       <c r="H63" s="60"/>
@@ -9351,7 +9351,7 @@
       <c r="D65" s="4"/>
       <c r="E65" s="58"/>
       <c r="F65" s="60">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="G65" s="60"/>
       <c r="H65" s="60"/>
@@ -9476,7 +9476,7 @@
       <c r="D67" s="4"/>
       <c r="E67" s="58"/>
       <c r="F67" s="60">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="G67" s="60"/>
       <c r="H67" s="60"/>
@@ -10432,7 +10432,7 @@
   </sheetPr>
   <dimension ref="A57:A69"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" view="pageBreakPreview" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageBreakPreview" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10459,7 +10459,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10588,41 +10588,41 @@
       <c r="C6" s="2">
         <v>0</v>
       </c>
-      <c r="D6" s="1">
-        <v>3870</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5716</v>
-      </c>
-      <c r="F6" s="1">
-        <v>6729</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5535</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5328</v>
-      </c>
-      <c r="I6" s="1">
-        <v>4130</v>
-      </c>
-      <c r="J6" s="1">
-        <v>820</v>
-      </c>
-      <c r="K6" s="1">
-        <v>7546.4</v>
-      </c>
-      <c r="L6" s="1">
-        <v>11528.5</v>
-      </c>
-      <c r="M6" s="1">
-        <v>10664</v>
-      </c>
-      <c r="N6" s="1">
-        <v>10762.5</v>
-      </c>
-      <c r="O6" s="1">
-        <v>11959.4</v>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="16"/>
@@ -10641,41 +10641,41 @@
       <c r="C7" s="2">
         <v>0</v>
       </c>
-      <c r="D7" s="1">
-        <v>34</v>
-      </c>
-      <c r="E7" s="1">
-        <v>62</v>
-      </c>
-      <c r="F7" s="1">
-        <v>77</v>
-      </c>
-      <c r="G7" s="1">
-        <v>43</v>
-      </c>
-      <c r="H7" s="1">
-        <v>44</v>
-      </c>
-      <c r="I7" s="1">
-        <v>42</v>
-      </c>
-      <c r="J7" s="1">
-        <v>4</v>
-      </c>
-      <c r="K7" s="1">
-        <v>81</v>
-      </c>
-      <c r="L7" s="1">
-        <v>87</v>
-      </c>
-      <c r="M7" s="1">
-        <v>108</v>
-      </c>
-      <c r="N7" s="1">
-        <v>106</v>
-      </c>
-      <c r="O7" s="1">
-        <v>120</v>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="16"/>
@@ -10753,41 +10753,41 @@
       <c r="C11" s="2">
         <v>0</v>
       </c>
-      <c r="D11" s="1">
-        <v>33</v>
-      </c>
-      <c r="E11" s="1">
-        <v>59</v>
-      </c>
-      <c r="F11" s="1">
-        <v>60</v>
-      </c>
-      <c r="G11" s="1">
-        <v>34</v>
-      </c>
-      <c r="H11" s="1">
-        <v>37</v>
-      </c>
-      <c r="I11" s="1">
-        <v>37</v>
-      </c>
-      <c r="J11" s="1">
-        <v>4</v>
-      </c>
-      <c r="K11" s="1">
-        <v>74</v>
-      </c>
-      <c r="L11" s="1">
-        <v>74</v>
-      </c>
-      <c r="M11" s="1">
-        <v>90</v>
-      </c>
-      <c r="N11" s="1">
-        <v>92</v>
-      </c>
-      <c r="O11" s="1">
-        <v>98</v>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="16"/>
@@ -10805,41 +10805,41 @@
       <c r="C12" s="2">
         <v>0</v>
       </c>
-      <c r="D12" s="1">
-        <v>113.82352941176499</v>
-      </c>
-      <c r="E12" s="1">
-        <v>92.193548387096797</v>
-      </c>
-      <c r="F12" s="1">
-        <v>87.389610389610397</v>
-      </c>
-      <c r="G12" s="1">
-        <v>128.720930232558</v>
-      </c>
-      <c r="H12" s="1">
-        <v>121.09090909090899</v>
-      </c>
-      <c r="I12" s="1">
-        <v>98.3333333333333</v>
-      </c>
-      <c r="J12" s="1">
-        <v>205</v>
-      </c>
-      <c r="K12" s="1">
-        <v>93.165432098765393</v>
-      </c>
-      <c r="L12" s="1">
-        <v>132.511494252874</v>
-      </c>
-      <c r="M12" s="1">
-        <v>98.740740740740705</v>
-      </c>
-      <c r="N12" s="1">
-        <v>101.53301886792499</v>
-      </c>
-      <c r="O12" s="1">
-        <v>99.661666666666704</v>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="16"/>
@@ -10895,25 +10895,25 @@
         <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>